<commit_message>
se eliminó un TestSuite que no se usaba se agrego la carpera Utilitarios/VPNConnect.exe
</commit_message>
<xml_diff>
--- a/PCQA/ExcelDatosCuentas.xlsx
+++ b/PCQA/ExcelDatosCuentas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD926373-D39B-4244-9A5A-9CC30141DDD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40153172-A9B0-4300-870A-5D6E3CD0B703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -236,6 +236,21 @@
   </si>
   <si>
     <t>Barredo</t>
+  </si>
+  <si>
+    <t>preproducciongestion.segurossura.com.ar</t>
+  </si>
+  <si>
+    <t>https://preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>PruebaRegre</t>
+  </si>
+  <si>
+    <t>AnswerRegre</t>
+  </si>
+  <si>
+    <t>MattioliRegre</t>
   </si>
 </sst>
 </file>
@@ -634,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,10 +719,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -716,13 +731,13 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H2">
-        <v>20300110</v>
+        <v>20300114</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>26</v>
@@ -743,7 +758,7 @@
         <v>28</v>
       </c>
       <c r="O2">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -751,10 +766,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -763,13 +778,13 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H3">
-        <v>20300111</v>
+        <v>20300115</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>26</v>
@@ -790,7 +805,7 @@
         <v>28</v>
       </c>
       <c r="O3">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1392,8 +1407,8 @@
     <hyperlink ref="C15" r:id="rId10" xr:uid="{C32C20E5-B653-474F-B15A-3BD438C33228}"/>
     <hyperlink ref="C16" r:id="rId11" xr:uid="{0B3716D5-CC64-46B6-904D-DBE8884C7365}"/>
     <hyperlink ref="C2" r:id="rId12" xr:uid="{E7266F27-FA55-47DD-9BDF-AC61C7F3CB6F}"/>
-    <hyperlink ref="C3" r:id="rId13" xr:uid="{12475220-8EE0-4BB2-9A02-00E7E88A2CB1}"/>
-    <hyperlink ref="C5" r:id="rId14" xr:uid="{B45CCA76-F8F7-4B4B-B4ED-E03E69453B51}"/>
+    <hyperlink ref="C5" r:id="rId13" xr:uid="{B45CCA76-F8F7-4B4B-B4ED-E03E69453B51}"/>
+    <hyperlink ref="C3" r:id="rId14" xr:uid="{A04A9E5E-09C2-4AA8-95D8-16223F2CDE39}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se organizaron items del repositorio se modif excel para hacer la regresion en preprod del R30
</commit_message>
<xml_diff>
--- a/PCQA/ExcelDatosCuentas.xlsx
+++ b/PCQA/ExcelDatosCuentas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399B1C14-820A-488D-88A4-6C2CFDE5227E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A26D49-5850-4411-A623-58DA6121F6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,13 +244,13 @@
     <t>https://preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
   </si>
   <si>
-    <t>AnswRegr</t>
-  </si>
-  <si>
-    <t>MattioliRegr</t>
-  </si>
-  <si>
-    <t>PruebaRegr</t>
+    <t>AnswRegrM</t>
+  </si>
+  <si>
+    <t>PruebaRegrM</t>
+  </si>
+  <si>
+    <t>MattioliRegrM</t>
   </si>
 </sst>
 </file>
@@ -650,7 +650,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,10 +734,10 @@
         <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H2">
-        <v>20300116</v>
+        <v>20300120</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>26</v>
@@ -755,7 +755,7 @@
         <v>28</v>
       </c>
       <c r="O2">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -775,13 +775,13 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" t="s">
         <v>71</v>
       </c>
-      <c r="G3" t="s">
-        <v>72</v>
-      </c>
       <c r="H3">
-        <v>20300117</v>
+        <v>20300121</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>26</v>
@@ -799,7 +799,7 @@
         <v>28</v>
       </c>
       <c r="O3">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se modif data para regresion en pre prod R31
</commit_message>
<xml_diff>
--- a/PCQA/ExcelDatosCuentas.xlsx
+++ b/PCQA/ExcelDatosCuentas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A40B4E-F9F6-491B-91B5-64B461B52000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD36842-B9E7-4C9F-A245-E176D0481E8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -244,13 +244,16 @@
     <t>https://preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
   </si>
   <si>
-    <t>AnswRegrM</t>
-  </si>
-  <si>
-    <t>PruebaRegrM</t>
-  </si>
-  <si>
-    <t>MattioliRegrM</t>
+    <t>AnswSmoke</t>
+  </si>
+  <si>
+    <t>SmokeMarzo</t>
+  </si>
+  <si>
+    <t>MattioliRegrAbril</t>
+  </si>
+  <si>
+    <t>PruebaRegrAbril</t>
   </si>
 </sst>
 </file>
@@ -649,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,16 +722,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
         <v>70</v>
@@ -778,10 +781,10 @@
         <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H3">
-        <v>20300123</v>
+        <v>20300124</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>26</v>
@@ -799,7 +802,7 @@
         <v>28</v>
       </c>
       <c r="O3">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1400,9 +1403,9 @@
     <hyperlink ref="C14" r:id="rId9" xr:uid="{16AFB98D-8486-4797-B18C-7D474A8D3925}"/>
     <hyperlink ref="C15" r:id="rId10" xr:uid="{C32C20E5-B653-474F-B15A-3BD438C33228}"/>
     <hyperlink ref="C16" r:id="rId11" xr:uid="{0B3716D5-CC64-46B6-904D-DBE8884C7365}"/>
-    <hyperlink ref="C2" r:id="rId12" xr:uid="{E7266F27-FA55-47DD-9BDF-AC61C7F3CB6F}"/>
-    <hyperlink ref="C5" r:id="rId13" xr:uid="{B45CCA76-F8F7-4B4B-B4ED-E03E69453B51}"/>
-    <hyperlink ref="C3" r:id="rId14" xr:uid="{A04A9E5E-09C2-4AA8-95D8-16223F2CDE39}"/>
+    <hyperlink ref="C5" r:id="rId12" xr:uid="{B45CCA76-F8F7-4B4B-B4ED-E03E69453B51}"/>
+    <hyperlink ref="C3" r:id="rId13" xr:uid="{A04A9E5E-09C2-4AA8-95D8-16223F2CDE39}"/>
+    <hyperlink ref="C2" r:id="rId14" xr:uid="{1797607C-F3AE-4C2F-91FE-51CC7A036B42}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
su modif Data para regresiones en Preprod
</commit_message>
<xml_diff>
--- a/PCQA/ExcelDatosCuentas.xlsx
+++ b/PCQA/ExcelDatosCuentas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD36842-B9E7-4C9F-A245-E176D0481E8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBF7775-8EFC-4379-9CC3-6E042BD45C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -238,22 +238,22 @@
     <t>Barredo</t>
   </si>
   <si>
-    <t>preproducciongestion.segurossura.com.ar</t>
-  </si>
-  <si>
-    <t>https://preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
-  </si>
-  <si>
-    <t>AnswSmoke</t>
-  </si>
-  <si>
-    <t>SmokeMarzo</t>
-  </si>
-  <si>
-    <t>MattioliRegrAbril</t>
-  </si>
-  <si>
-    <t>PruebaRegrAbril</t>
+    <t>AnswerDos</t>
+  </si>
+  <si>
+    <t>PruebaDos</t>
+  </si>
+  <si>
+    <t>AnswRegrAbrilDos</t>
+  </si>
+  <si>
+    <t>AnsRegrAbrilDos</t>
+  </si>
+  <si>
+    <t>MattioliRegrAbrilDos</t>
+  </si>
+  <si>
+    <t>PruebaRegrAbrilDos</t>
   </si>
 </sst>
 </file>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,16 +722,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
         <v>70</v>
@@ -740,7 +740,7 @@
         <v>71</v>
       </c>
       <c r="H2">
-        <v>20300122</v>
+        <v>20300126</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>26</v>
@@ -758,7 +758,7 @@
         <v>28</v>
       </c>
       <c r="O2">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -766,10 +766,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -784,7 +784,7 @@
         <v>73</v>
       </c>
       <c r="H3">
-        <v>20300124</v>
+        <v>20300127</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>26</v>
@@ -802,7 +802,7 @@
         <v>28</v>
       </c>
       <c r="O3">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1007,13 +1007,13 @@
         <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="H8">
-        <v>20300100</v>
+        <v>20300101</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>26</v>
@@ -1034,7 +1034,7 @@
         <v>28</v>
       </c>
       <c r="O8">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1404,8 +1404,8 @@
     <hyperlink ref="C15" r:id="rId10" xr:uid="{C32C20E5-B653-474F-B15A-3BD438C33228}"/>
     <hyperlink ref="C16" r:id="rId11" xr:uid="{0B3716D5-CC64-46B6-904D-DBE8884C7365}"/>
     <hyperlink ref="C5" r:id="rId12" xr:uid="{B45CCA76-F8F7-4B4B-B4ED-E03E69453B51}"/>
-    <hyperlink ref="C3" r:id="rId13" xr:uid="{A04A9E5E-09C2-4AA8-95D8-16223F2CDE39}"/>
-    <hyperlink ref="C2" r:id="rId14" xr:uid="{1797607C-F3AE-4C2F-91FE-51CC7A036B42}"/>
+    <hyperlink ref="C2" r:id="rId13" xr:uid="{EA537629-037E-4A78-9ABC-629425471EFD}"/>
+    <hyperlink ref="C3" r:id="rId14" xr:uid="{BB5826D9-5E84-44D6-B660-4FB30DCA39F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se arregló el script crear cuenta compañia para la seleccion de dirección y se modifica data para la creacion de cuentas en pre prod para la regresion R33
</commit_message>
<xml_diff>
--- a/PCQA/ExcelDatosCuentas.xlsx
+++ b/PCQA/ExcelDatosCuentas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBF7775-8EFC-4379-9CC3-6E042BD45C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC206AE2-17C4-4897-886D-A518C02BE5E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,16 +244,16 @@
     <t>PruebaDos</t>
   </si>
   <si>
-    <t>AnswRegrAbrilDos</t>
-  </si>
-  <si>
-    <t>AnsRegrAbrilDos</t>
-  </si>
-  <si>
-    <t>MattioliRegrAbrilDos</t>
-  </si>
-  <si>
-    <t>PruebaRegrAbrilDos</t>
+    <t>AnswRegrJunioUno</t>
+  </si>
+  <si>
+    <t>AnsRegrJunioUno</t>
+  </si>
+  <si>
+    <t>MattioliRegrJunioUno</t>
+  </si>
+  <si>
+    <t>PruebaRegrJunioUno</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +740,7 @@
         <v>71</v>
       </c>
       <c r="H2">
-        <v>20300126</v>
+        <v>20300128</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>26</v>
@@ -758,7 +758,7 @@
         <v>28</v>
       </c>
       <c r="O2">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
         <v>73</v>
       </c>
       <c r="H3">
-        <v>20300127</v>
+        <v>20300128</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>26</v>
@@ -802,7 +802,7 @@
         <v>28</v>
       </c>
       <c r="O3">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>